<commit_message>
COST and other updates
</commit_message>
<xml_diff>
--- a/AVGO.xlsx
+++ b/AVGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Shkreli - DL\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D78B31C-CAEF-4A8A-B560-382CA715EE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A71D4FF-2404-40D7-940E-718802EC9CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="3670" windowWidth="18690" windowHeight="15380" activeTab="1" xr2:uid="{70329CC5-8756-4BA4-A5C1-E709DAADAB52}"/>
+    <workbookView xWindow="16920" yWindow="2060" windowWidth="20920" windowHeight="16150" xr2:uid="{70329CC5-8756-4BA4-A5C1-E709DAADAB52}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -353,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -381,11 +381,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -412,16 +409,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>32525</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>40462</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>13260</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>32525</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>40462</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>138712</xdr:rowOff>
+      <xdr:rowOff>125452</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -436,8 +433,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6287275" y="13260"/>
-          <a:ext cx="0" cy="10634702"/>
+          <a:off x="7454087" y="0"/>
+          <a:ext cx="0" cy="10944265"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -832,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9849E712-1B47-42A3-A902-777D3000824F}">
   <dimension ref="B2:K17"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -843,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>176.75</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -869,7 +866,7 @@
       </c>
       <c r="J4" s="5">
         <f>+J2*J3</f>
-        <v>825524.32267024997</v>
+        <v>906091.76010199997</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -909,7 +906,7 @@
       </c>
       <c r="J7" s="2">
         <f>+J4-J5+J6</f>
-        <v>887128.32267024997</v>
+        <v>967695.76010199997</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -972,11 +969,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E0775-30FD-4D74-BE40-C6F63DB74CF0}">
   <dimension ref="A1:X70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1265,10 +1262,11 @@
         <v>13072</v>
       </c>
       <c r="K9" s="10">
-        <f>+K7+K8</f>
-        <v>14072</v>
-      </c>
-      <c r="L9" s="12"/>
+        <v>14054</v>
+      </c>
+      <c r="L9" s="10">
+        <v>14916</v>
+      </c>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
@@ -1323,8 +1321,10 @@
         <v>3133</v>
       </c>
       <c r="K10" s="8">
-        <f>+K9-K11</f>
-        <v>3377.2800000000007</v>
+        <v>3399</v>
+      </c>
+      <c r="L10" s="8">
+        <v>3273</v>
       </c>
       <c r="T10" s="8">
         <v>6555</v>
@@ -1378,10 +1378,13 @@
         <v>9939</v>
       </c>
       <c r="K11" s="8">
-        <f>+K9*0.76</f>
-        <v>10694.72</v>
-      </c>
-      <c r="L11" s="8"/>
+        <f>+K9-K10</f>
+        <v>10655</v>
+      </c>
+      <c r="L11" s="8">
+        <f>+L9-L10</f>
+        <v>11643</v>
+      </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -1436,8 +1439,10 @@
         <v>2353</v>
       </c>
       <c r="K12" s="8">
-        <f>+H12</f>
-        <v>2308</v>
+        <v>2234</v>
+      </c>
+      <c r="L12" s="8">
+        <v>2253</v>
       </c>
       <c r="T12" s="8">
         <v>4854</v>
@@ -1483,8 +1488,10 @@
         <v>1100</v>
       </c>
       <c r="K13" s="8">
-        <f>+H13</f>
-        <v>1572</v>
+        <v>1010</v>
+      </c>
+      <c r="L13" s="8">
+        <v>949</v>
       </c>
       <c r="T13" s="8">
         <v>1347</v>
@@ -1506,7 +1513,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="8">
-        <f t="shared" ref="C14:K14" si="1">+C12+C13</f>
+        <f t="shared" ref="C14:L14" si="1">+C12+C13</f>
         <v>1567</v>
       </c>
       <c r="D14" s="8">
@@ -1539,7 +1546,11 @@
       </c>
       <c r="K14" s="8">
         <f t="shared" si="1"/>
-        <v>3880</v>
+        <v>3244</v>
+      </c>
+      <c r="L14" s="8">
+        <f t="shared" si="1"/>
+        <v>3202</v>
       </c>
       <c r="T14" s="8">
         <f t="shared" ref="T14:U14" si="2">+T13+T12</f>
@@ -1563,7 +1574,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="8">
-        <f t="shared" ref="C15:K15" si="3">+C11-C14</f>
+        <f t="shared" ref="C15:L15" si="3">+C11-C14</f>
         <v>5065</v>
       </c>
       <c r="D15" s="8">
@@ -1596,7 +1607,11 @@
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>6814.7199999999993</v>
+        <v>7411</v>
+      </c>
+      <c r="L15" s="8">
+        <f t="shared" si="3"/>
+        <v>8441</v>
       </c>
       <c r="T15" s="8">
         <f t="shared" ref="T15:U15" si="4">+T11-T14</f>
@@ -1652,8 +1667,12 @@
         <v>-982</v>
       </c>
       <c r="K16" s="8">
-        <f>+J16</f>
-        <v>-982</v>
+        <f>-916+52</f>
+        <v>-864</v>
+      </c>
+      <c r="L16" s="3">
+        <f>-873+103</f>
+        <v>-770</v>
       </c>
       <c r="T16" s="8">
         <f>-1885+131</f>
@@ -1677,7 +1696,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="8">
-        <f t="shared" ref="C17:K17" si="5">+C15+C16</f>
+        <f t="shared" ref="C17:L17" si="5">+C15+C16</f>
         <v>4699</v>
       </c>
       <c r="D17" s="8">
@@ -1710,7 +1729,11 @@
       </c>
       <c r="K17" s="8">
         <f t="shared" si="5"/>
-        <v>5832.7199999999993</v>
+        <v>6547</v>
+      </c>
+      <c r="L17" s="8">
+        <f t="shared" si="5"/>
+        <v>7671</v>
       </c>
       <c r="T17" s="8">
         <f>+T15+T16</f>
@@ -1749,7 +1772,8 @@
         <v>443</v>
       </c>
       <c r="H18" s="8">
-        <v>68</v>
+        <f>68+735</f>
+        <v>803</v>
       </c>
       <c r="I18" s="8">
         <v>-116</v>
@@ -1758,10 +1782,13 @@
         <v>4238</v>
       </c>
       <c r="K18" s="8">
-        <f>+K17*0.1</f>
-        <v>583.27199999999993</v>
-      </c>
-      <c r="L18" s="8"/>
+        <f>-442+1506</f>
+        <v>1064</v>
+      </c>
+      <c r="L18" s="8">
+        <f>-12+1286</f>
+        <v>1274</v>
+      </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1792,7 +1819,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="8">
-        <f t="shared" ref="C19:K19" si="6">+C17-C18</f>
+        <f t="shared" ref="C19:L19" si="6">+C17-C18</f>
         <v>4438</v>
       </c>
       <c r="D19" s="8">
@@ -1813,7 +1840,7 @@
       </c>
       <c r="H19" s="8">
         <f t="shared" si="6"/>
-        <v>4158</v>
+        <v>3423</v>
       </c>
       <c r="I19" s="8">
         <f t="shared" si="6"/>
@@ -1825,7 +1852,11 @@
       </c>
       <c r="K19" s="8">
         <f t="shared" si="6"/>
-        <v>5249.4479999999994</v>
+        <v>5483</v>
+      </c>
+      <c r="L19" s="8">
+        <f t="shared" si="6"/>
+        <v>6397</v>
       </c>
       <c r="T19" s="10">
         <f>+T17-T18</f>
@@ -1849,7 +1880,7 @@
         <v>75</v>
       </c>
       <c r="C20" s="11">
-        <f t="shared" ref="C20:K20" si="7">+C19/C21</f>
+        <f t="shared" ref="C20:L20" si="7">+C19/C21</f>
         <v>1.0344988344988344</v>
       </c>
       <c r="D20" s="11">
@@ -1870,7 +1901,7 @@
       </c>
       <c r="H20" s="11">
         <f t="shared" si="7"/>
-        <v>0.89036402569593143</v>
+        <v>0.73297644539614559</v>
       </c>
       <c r="I20" s="11">
         <f t="shared" si="7"/>
@@ -1882,7 +1913,11 @@
       </c>
       <c r="K20" s="11">
         <f t="shared" si="7"/>
-        <v>1.1257662449067123</v>
+        <v>1.1356669428334714</v>
+      </c>
+      <c r="L20" s="11">
+        <f t="shared" si="7"/>
+        <v>1.3227874276261373</v>
       </c>
       <c r="T20" s="11">
         <f>+T19/T21</f>
@@ -1931,8 +1966,10 @@
         <v>4663</v>
       </c>
       <c r="K21" s="8">
-        <f>+J21</f>
-        <v>4663</v>
+        <v>4828</v>
+      </c>
+      <c r="L21" s="8">
+        <v>4836</v>
       </c>
       <c r="T21" s="8">
         <v>4290</v>
@@ -1971,9 +2008,12 @@
       </c>
       <c r="K25" s="9">
         <f>+K9/G9-1</f>
-        <v>0.51393222162452923</v>
-      </c>
-      <c r="L25" s="9"/>
+        <v>0.51199569661108124</v>
+      </c>
+      <c r="L25" s="9">
+        <f>+L9/H9-1</f>
+        <v>0.24705292199648854</v>
+      </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
@@ -2031,7 +2071,11 @@
       </c>
       <c r="K26" s="9">
         <f>+K11/K9</f>
-        <v>0.76</v>
+        <v>0.75814714671979511</v>
+      </c>
+      <c r="L26" s="9">
+        <f>+L11/L9</f>
+        <v>0.78057119871279168</v>
       </c>
       <c r="T26" s="9">
         <f>+T11/T9</f>
@@ -2088,7 +2132,11 @@
       </c>
       <c r="K27" s="9">
         <f>+K15/K9</f>
-        <v>0.48427515633882884</v>
+        <v>0.52732318201223849</v>
+      </c>
+      <c r="L27" s="9">
+        <f>+L15/L9</f>
+        <v>0.56590238669884685</v>
       </c>
       <c r="T27" s="9">
         <f>+T15/T9</f>
@@ -2644,7 +2692,7 @@
       </c>
       <c r="H47" s="8">
         <f>+H19</f>
-        <v>4158</v>
+        <v>3423</v>
       </c>
       <c r="I47" s="8">
         <f>+I19</f>
@@ -2659,10 +2707,10 @@
       <c r="B48" t="s">
         <v>40</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="8">
         <v>1325</v>
       </c>
-      <c r="I48" s="15">
+      <c r="I48" s="8">
         <v>2121</v>
       </c>
       <c r="J48" s="8">

</xml_diff>